<commit_message>
added uml and workspace with sample code
</commit_message>
<xml_diff>
--- a/doc/Projektplan.xlsx
+++ b/doc/Projektplan.xlsx
@@ -167,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +329,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="0"/>
+        <bgColor theme="7"/>
       </patternFill>
     </fill>
   </fills>
@@ -367,7 +373,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,81 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
@@ -507,6 +439,84 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
@@ -802,7 +812,7 @@
   <dimension ref="D3:AK24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,126 +825,126 @@
   <sheetData>
     <row r="3" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="32"/>
-      <c r="P3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="4:37" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="4"/>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="48"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="47" t="s">
+      <c r="X4" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="58"/>
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="58"/>
       <c r="AF4" s="7"/>
-      <c r="AG4" s="50" t="s">
+      <c r="AG4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
-      <c r="AJ4" s="50"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
       <c r="AK4" s="12"/>
     </row>
     <row r="5" spans="4:37" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="45" t="s">
+      <c r="G5" s="51"/>
+      <c r="H5" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="45" t="s">
+      <c r="I5" s="51"/>
+      <c r="J5" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="46" t="s">
+      <c r="K5" s="51"/>
+      <c r="L5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="46"/>
-      <c r="N5" s="53" t="s">
+      <c r="M5" s="57"/>
+      <c r="N5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="45" t="s">
+      <c r="P5" s="51"/>
+      <c r="Q5" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="40"/>
-      <c r="S5" s="45" t="s">
+      <c r="R5" s="51"/>
+      <c r="S5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="40"/>
-      <c r="U5" s="46" t="s">
+      <c r="T5" s="51"/>
+      <c r="U5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="V5" s="46"/>
-      <c r="W5" s="49" t="s">
+      <c r="V5" s="57"/>
+      <c r="W5" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="39" t="s">
+      <c r="X5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="45" t="s">
+      <c r="Y5" s="51"/>
+      <c r="Z5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="45" t="s">
+      <c r="AA5" s="51"/>
+      <c r="AB5" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="46" t="s">
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="51" t="s">
+      <c r="AE5" s="57"/>
+      <c r="AF5" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="AG5" s="39" t="s">
+      <c r="AG5" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="AH5" s="40"/>
-      <c r="AI5" s="46" t="s">
+      <c r="AH5" s="51"/>
+      <c r="AI5" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="52" t="s">
+      <c r="AJ5" s="57"/>
+      <c r="AK5" s="63" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="4:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="52" t="s">
         <v>17</v>
       </c>
       <c r="E6" t="s">
@@ -948,7 +958,7 @@
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
       <c r="M6" s="16"/>
-      <c r="N6" s="53"/>
+      <c r="N6" s="64"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="1"/>
@@ -957,7 +967,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
-      <c r="W6" s="49"/>
+      <c r="W6" s="60"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
@@ -966,15 +976,15 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="51"/>
+      <c r="AF6" s="62"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="8"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
-      <c r="AK6" s="52"/>
+      <c r="AK6" s="63"/>
     </row>
     <row r="7" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D7" s="41"/>
+      <c r="D7" s="52"/>
       <c r="E7" t="s">
         <v>27</v>
       </c>
@@ -982,21 +992,21 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="53"/>
-      <c r="P7" s="66"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="64"/>
+      <c r="P7" s="40"/>
       <c r="R7" s="11"/>
-      <c r="W7" s="49"/>
+      <c r="W7" s="60"/>
       <c r="AA7" s="11"/>
-      <c r="AF7" s="51"/>
+      <c r="AF7" s="62"/>
       <c r="AH7" s="10"/>
-      <c r="AK7" s="52"/>
+      <c r="AK7" s="63"/>
     </row>
     <row r="8" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="53" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
@@ -1007,20 +1017,20 @@
       <c r="H8" s="10"/>
       <c r="I8" s="11"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="53"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="18"/>
-      <c r="W8" s="49"/>
+      <c r="W8" s="60"/>
       <c r="AA8" s="11"/>
-      <c r="AF8" s="51"/>
+      <c r="AF8" s="62"/>
       <c r="AH8" s="10"/>
-      <c r="AK8" s="52"/>
+      <c r="AK8" s="63"/>
     </row>
     <row r="9" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D9" s="42"/>
+      <c r="D9" s="53"/>
       <c r="E9" t="s">
         <v>27</v>
       </c>
@@ -1028,19 +1038,20 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="11"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="53"/>
-      <c r="P9" s="60"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="64"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
       <c r="R9" s="11"/>
-      <c r="W9" s="49"/>
+      <c r="W9" s="60"/>
       <c r="AA9" s="11"/>
-      <c r="AF9" s="51"/>
+      <c r="AF9" s="62"/>
       <c r="AH9" s="10"/>
-      <c r="AK9" s="52"/>
+      <c r="AK9" s="63"/>
     </row>
     <row r="10" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="54" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
@@ -1050,27 +1061,27 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="11"/>
-      <c r="N10" s="53"/>
+      <c r="N10" s="64"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
+      <c r="R10" s="21"/>
       <c r="S10" s="20"/>
       <c r="T10" s="20"/>
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
-      <c r="W10" s="49"/>
+      <c r="W10" s="60"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="20"/>
       <c r="Z10" s="20"/>
       <c r="AA10" s="21"/>
       <c r="AB10" s="20"/>
       <c r="AD10" s="20"/>
-      <c r="AF10" s="51"/>
+      <c r="AF10" s="62"/>
       <c r="AH10" s="10"/>
-      <c r="AK10" s="52"/>
+      <c r="AK10" s="63"/>
     </row>
     <row r="11" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D11" s="43"/>
+      <c r="D11" s="54"/>
       <c r="E11" t="s">
         <v>27</v>
       </c>
@@ -1078,17 +1089,18 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="11"/>
-      <c r="N11" s="53"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="11"/>
-      <c r="W11" s="49"/>
+      <c r="N11" s="64"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="70"/>
+      <c r="W11" s="60"/>
       <c r="AA11" s="11"/>
-      <c r="AF11" s="51"/>
+      <c r="AF11" s="62"/>
       <c r="AH11" s="10"/>
-      <c r="AK11" s="52"/>
+      <c r="AK11" s="63"/>
     </row>
     <row r="12" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E12" t="s">
@@ -1098,12 +1110,12 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="11"/>
-      <c r="N12" s="53"/>
+      <c r="N12" s="64"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="24"/>
       <c r="T12" s="23"/>
       <c r="U12" s="23"/>
-      <c r="W12" s="49"/>
+      <c r="W12" s="60"/>
       <c r="X12" s="23"/>
       <c r="Y12" s="23"/>
       <c r="Z12" s="23"/>
@@ -1112,13 +1124,13 @@
       <c r="AC12" s="23"/>
       <c r="AD12" s="23"/>
       <c r="AE12" s="23"/>
-      <c r="AF12" s="51"/>
+      <c r="AF12" s="62"/>
       <c r="AH12" s="29"/>
       <c r="AI12" s="29"/>
-      <c r="AK12" s="52"/>
+      <c r="AK12" s="63"/>
     </row>
     <row r="13" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D13" s="44"/>
+      <c r="D13" s="55"/>
       <c r="E13" t="s">
         <v>27</v>
       </c>
@@ -1126,17 +1138,16 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="11"/>
-      <c r="N13" s="53"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="11"/>
-      <c r="W13" s="49"/>
+      <c r="N13" s="64"/>
+      <c r="R13" s="69"/>
+      <c r="W13" s="60"/>
       <c r="AA13" s="11"/>
-      <c r="AF13" s="51"/>
+      <c r="AF13" s="62"/>
       <c r="AH13" s="10"/>
-      <c r="AK13" s="52"/>
+      <c r="AK13" s="63"/>
     </row>
     <row r="14" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
@@ -1146,24 +1157,24 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="11"/>
-      <c r="N14" s="53"/>
+      <c r="N14" s="64"/>
       <c r="P14" s="25"/>
       <c r="R14" s="11"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
-      <c r="W14" s="49"/>
+      <c r="W14" s="60"/>
       <c r="Y14" s="25"/>
       <c r="AA14" s="26"/>
       <c r="AC14" s="25"/>
       <c r="AE14" s="25"/>
-      <c r="AF14" s="51"/>
+      <c r="AF14" s="62"/>
       <c r="AG14" s="25"/>
       <c r="AH14" s="27"/>
       <c r="AI14" s="27"/>
-      <c r="AK14" s="52"/>
+      <c r="AK14" s="63"/>
     </row>
     <row r="15" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D15" s="33"/>
+      <c r="D15" s="44"/>
       <c r="E15" t="s">
         <v>27</v>
       </c>
@@ -1171,17 +1182,16 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="11"/>
-      <c r="N15" s="53"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="11"/>
-      <c r="W15" s="49"/>
+      <c r="N15" s="64"/>
+      <c r="R15" s="68"/>
+      <c r="W15" s="60"/>
       <c r="AA15" s="11"/>
-      <c r="AF15" s="51"/>
+      <c r="AF15" s="62"/>
       <c r="AH15" s="10"/>
-      <c r="AK15" s="52"/>
+      <c r="AK15" s="63"/>
     </row>
     <row r="16" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="45" t="s">
         <v>22</v>
       </c>
       <c r="E16" t="s">
@@ -1191,17 +1201,17 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="11"/>
-      <c r="N16" s="53"/>
+      <c r="N16" s="64"/>
       <c r="R16" s="11"/>
-      <c r="W16" s="49"/>
+      <c r="W16" s="60"/>
       <c r="AA16" s="11"/>
-      <c r="AF16" s="51"/>
+      <c r="AF16" s="62"/>
       <c r="AH16" s="10"/>
       <c r="AJ16" s="28"/>
-      <c r="AK16" s="52"/>
+      <c r="AK16" s="63"/>
     </row>
     <row r="17" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D17" s="34"/>
+      <c r="D17" s="45"/>
       <c r="E17" t="s">
         <v>27</v>
       </c>
@@ -1209,16 +1219,16 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="11"/>
-      <c r="N17" s="53"/>
+      <c r="N17" s="64"/>
       <c r="R17" s="11"/>
-      <c r="W17" s="49"/>
+      <c r="W17" s="60"/>
       <c r="AA17" s="11"/>
-      <c r="AF17" s="51"/>
+      <c r="AF17" s="62"/>
       <c r="AH17" s="10"/>
-      <c r="AK17" s="52"/>
+      <c r="AK17" s="63"/>
     </row>
     <row r="18" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="46" t="s">
         <v>23</v>
       </c>
       <c r="E18" t="s">
@@ -1228,24 +1238,26 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="11"/>
-      <c r="N18" s="53"/>
+      <c r="N18" s="64"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="10"/>
       <c r="R18" s="30"/>
       <c r="S18" s="22"/>
       <c r="U18" s="22"/>
-      <c r="W18" s="49"/>
+      <c r="W18" s="60"/>
       <c r="X18" s="22"/>
       <c r="Z18" s="22"/>
       <c r="AA18" s="11"/>
       <c r="AB18" s="22"/>
       <c r="AD18" s="22"/>
       <c r="AE18" s="22"/>
-      <c r="AF18" s="51"/>
+      <c r="AF18" s="62"/>
       <c r="AG18" s="22"/>
       <c r="AH18" s="22"/>
-      <c r="AK18" s="52"/>
+      <c r="AK18" s="63"/>
     </row>
     <row r="19" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D19" s="35"/>
+      <c r="D19" s="46"/>
       <c r="E19" t="s">
         <v>27</v>
       </c>
@@ -1253,16 +1265,17 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="11"/>
-      <c r="N19" s="53"/>
-      <c r="R19" s="11"/>
-      <c r="W19" s="49"/>
+      <c r="N19" s="64"/>
+      <c r="P19" s="43"/>
+      <c r="R19" s="72"/>
+      <c r="W19" s="60"/>
       <c r="AA19" s="11"/>
-      <c r="AF19" s="51"/>
+      <c r="AF19" s="62"/>
       <c r="AH19" s="10"/>
-      <c r="AK19" s="52"/>
+      <c r="AK19" s="63"/>
     </row>
     <row r="20" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E20" t="s">
@@ -1276,49 +1289,49 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="53"/>
+      <c r="N20" s="64"/>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="14"/>
       <c r="T20" s="15"/>
       <c r="V20" s="15"/>
-      <c r="W20" s="49"/>
+      <c r="W20" s="60"/>
       <c r="Y20" s="15"/>
       <c r="AA20" s="14"/>
       <c r="AC20" s="15"/>
       <c r="AE20" s="15"/>
-      <c r="AF20" s="51"/>
+      <c r="AF20" s="62"/>
       <c r="AH20" s="13"/>
       <c r="AI20" s="15"/>
       <c r="AJ20" s="15"/>
-      <c r="AK20" s="52"/>
+      <c r="AK20" s="63"/>
     </row>
     <row r="21" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D21" s="36"/>
+      <c r="D21" s="47"/>
       <c r="E21" t="s">
         <v>27</v>
       </c>
       <c r="F21" s="10"/>
-      <c r="G21" s="64"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="53"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="64"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
       <c r="R21" s="11"/>
-      <c r="W21" s="49"/>
+      <c r="W21" s="60"/>
       <c r="AA21" s="11"/>
-      <c r="AF21" s="51"/>
+      <c r="AF21" s="62"/>
       <c r="AH21" s="10"/>
-      <c r="AK21" s="52"/>
+      <c r="AK21" s="63"/>
     </row>
     <row r="22" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="48" t="s">
         <v>25</v>
       </c>
       <c r="E22" t="s">
@@ -1329,77 +1342,77 @@
       <c r="H22" s="10"/>
       <c r="I22" s="11"/>
       <c r="M22" s="31"/>
-      <c r="N22" s="53"/>
+      <c r="N22" s="64"/>
       <c r="R22" s="11"/>
-      <c r="W22" s="49"/>
+      <c r="W22" s="60"/>
       <c r="AA22" s="11"/>
-      <c r="AF22" s="51"/>
+      <c r="AF22" s="62"/>
       <c r="AH22" s="10"/>
-      <c r="AK22" s="52"/>
+      <c r="AK22" s="63"/>
     </row>
     <row r="23" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D23" s="37"/>
+      <c r="D23" s="48"/>
       <c r="E23" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="63"/>
+      <c r="G23" s="37"/>
       <c r="H23" s="10"/>
       <c r="I23" s="11"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="53"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="64"/>
       <c r="R23" s="11"/>
-      <c r="W23" s="49"/>
+      <c r="W23" s="60"/>
       <c r="AA23" s="11"/>
-      <c r="AF23" s="51"/>
+      <c r="AF23" s="62"/>
       <c r="AH23" s="10"/>
-      <c r="AK23" s="52"/>
+      <c r="AK23" s="63"/>
     </row>
     <row r="24" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="56" t="s">
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="O24" s="54" t="s">
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="O24" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="56" t="s">
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="X24" s="54" t="s">
+      <c r="T24" s="67"/>
+      <c r="U24" s="67"/>
+      <c r="V24" s="67"/>
+      <c r="X24" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="Y24" s="54"/>
-      <c r="Z24" s="54"/>
-      <c r="AA24" s="55"/>
-      <c r="AB24" s="56" t="s">
+      <c r="Y24" s="65"/>
+      <c r="Z24" s="65"/>
+      <c r="AA24" s="66"/>
+      <c r="AB24" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="AC24" s="56"/>
-      <c r="AD24" s="56"/>
-      <c r="AE24" s="56"/>
-      <c r="AF24" s="51"/>
-      <c r="AG24" s="54" t="s">
+      <c r="AC24" s="67"/>
+      <c r="AD24" s="67"/>
+      <c r="AE24" s="67"/>
+      <c r="AF24" s="62"/>
+      <c r="AG24" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="AH24" s="54"/>
-      <c r="AI24" s="54"/>
-      <c r="AJ24" s="55"/>
-      <c r="AK24" s="52"/>
+      <c r="AH24" s="65"/>
+      <c r="AI24" s="65"/>
+      <c r="AJ24" s="66"/>
+      <c r="AK24" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="38">

</xml_diff>